<commit_message>
update android test case
</commit_message>
<xml_diff>
--- a/Documents/Android_Test_cases.xlsx
+++ b/Documents/Android_Test_cases.xlsx
@@ -5,21 +5,29 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ministore\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="0" showVerticalScroll="0" xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5916"/>
+    <workbookView showHorizontalScroll="0" showVerticalScroll="0" xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5916" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestCase" sheetId="17" r:id="rId1"/>
+    <sheet name="Home-Trang chủ" sheetId="19" r:id="rId2"/>
+    <sheet name="Login-Đăng nhập" sheetId="20" r:id="rId3"/>
+    <sheet name="Signup-Đăng ký" sheetId="21" r:id="rId4"/>
+    <sheet name="Cart-Giỏ hàng" sheetId="22" r:id="rId5"/>
+    <sheet name="Category-Danh mục" sheetId="23" r:id="rId6"/>
+    <sheet name="Account-Tài khoản" sheetId="24" r:id="rId7"/>
+    <sheet name="Shipper-Giao hàng" sheetId="25" r:id="rId8"/>
+    <sheet name="Bug TC_SU_002" sheetId="18" r:id="rId9"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="221">
   <si>
     <t>Thiết kế</t>
   </si>
@@ -282,17 +290,456 @@
     <t>Hủy giao</t>
   </si>
   <si>
-    <t>Thông báo thành công. Đơn hàng chuyển qua trạng thái đã giao</t>
-  </si>
-  <si>
     <t>Thông báo thành công. Đơn hàng chuyển qua trạng thái đã hủy</t>
+  </si>
+  <si>
+    <t>Hiển thị sai message</t>
+  </si>
+  <si>
+    <t>Lỗi sai message</t>
+  </si>
+  <si>
+    <t>Mở dialog xác nhận. Thông báo thành công. Đơn hàng chuyển qua trạng thái đã giao</t>
+  </si>
+  <si>
+    <t>Testcase ID</t>
+  </si>
+  <si>
+    <t>Test Scenario</t>
+  </si>
+  <si>
+    <t>Test cases</t>
+  </si>
+  <si>
+    <t>Pre-Condition</t>
+  </si>
+  <si>
+    <t>Data Input</t>
+  </si>
+  <si>
+    <t>Step procedure</t>
+  </si>
+  <si>
+    <t>Expected result</t>
+  </si>
+  <si>
+    <t>Actual results</t>
+  </si>
+  <si>
+    <t>Version/Divice</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>UI/UX</t>
+  </si>
+  <si>
+    <t>Samsung</t>
+  </si>
+  <si>
+    <t>Iphone</t>
+  </si>
+  <si>
+    <t>TC_H_001</t>
+  </si>
+  <si>
+    <t>TC_H_002</t>
+  </si>
+  <si>
+    <t>TC_H_003</t>
+  </si>
+  <si>
+    <t>TC_H_004</t>
+  </si>
+  <si>
+    <t>TC_H_005</t>
+  </si>
+  <si>
+    <t>Hiển thị đúng</t>
+  </si>
+  <si>
+    <t>Kiểm tra home có hiển thị đúng những sản phẩm mới ở mục new product hay không</t>
+  </si>
+  <si>
+    <t>1. Mở ứng dụng
+2.Người dùng ở trang khác trang Home</t>
+  </si>
+  <si>
+    <t>Kiểm tra home có hiển thị đúng những sản phẩm bán chạy ở mục popular product hay không</t>
+  </si>
+  <si>
+    <t>Thêm sản phẩm từ trang chủ vào giỏ hàng</t>
+  </si>
+  <si>
+    <t>Kiểm tra xem có thêm được sản phẩm vào giỏ hàng từ trang home hay không</t>
+  </si>
+  <si>
+    <t>Đã đăng nhập</t>
+  </si>
+  <si>
+    <t>1. Người dùng ở trang home
+2.Người dùng chọn button "+" của sản phẩm</t>
+  </si>
+  <si>
+    <t>Sản phẩm được thêm vào cart</t>
+  </si>
+  <si>
+    <t>Chi tiết sản phẩm</t>
+  </si>
+  <si>
+    <t>Kiểm tra khi nhấn vào sản phẩm có xem được chi tiết thông tin sản phẩm hay không</t>
+  </si>
+  <si>
+    <t>1. Người dùng ở trang home
+2.Người dùng chọn vào vùng 1 sản phẩm bất kỳ</t>
+  </si>
+  <si>
+    <t>Chuyển màn hình hiển thị thông tin chi tiết sản phẩm</t>
+  </si>
+  <si>
+    <t>TC_H_006</t>
+  </si>
+  <si>
+    <t>Tìm kiếm sản phẩm</t>
+  </si>
+  <si>
+    <t>Kiểm tra xem giao diện có thiết kế giống tài liệu thiết kế hay không</t>
+  </si>
+  <si>
+    <t>Kiểm tra xem chức năng tìm kiếm sản phẩm</t>
+  </si>
+  <si>
+    <t>Bút</t>
+  </si>
+  <si>
+    <t>1. Người dùng ở trang home
+2.Người dùng chọn vào thanh tìm kiếm
+3. Người dùng nhập "Bút"</t>
+  </si>
+  <si>
+    <t>Hiển thị các sản phẩm có liên quan đến "Bút"</t>
+  </si>
+  <si>
+    <t>TC_LG_001</t>
+  </si>
+  <si>
+    <t>TC_LG_002</t>
+  </si>
+  <si>
+    <t>TC_LG_003</t>
+  </si>
+  <si>
+    <t>TC_LG_004</t>
+  </si>
+  <si>
+    <t>TC_LG_005</t>
+  </si>
+  <si>
+    <t>Kiểm tra để trống username, password</t>
+  </si>
+  <si>
+    <t>1. Mở ứng dụng
+2.Chọn màn hình account
+3.Chọn login</t>
+  </si>
+  <si>
+    <t>Kiểm tra sai username, password</t>
+  </si>
+  <si>
+    <t>1. Nhập data input
+2.Nhấn button login</t>
+  </si>
+  <si>
+    <t>Kiểm tra đăng nhập thành công</t>
+  </si>
+  <si>
+    <t>Quên mật khẩu</t>
+  </si>
+  <si>
+    <t>1. Ở màn hình login
+2.Nhấn text forget password</t>
+  </si>
+  <si>
+    <t>1.Chuyển màn hình yêu cầu nhập tên username
+2. Chọn phương thức gửi mã OTP
+3. Nhập mã OTP
+4. Nếu đúng mã OTP sẽ nhập mật khẩu mới</t>
+  </si>
+  <si>
+    <t>khachung123</t>
+  </si>
+  <si>
+    <t>Kiểm tra chức năng quên mật khẩu</t>
+  </si>
+  <si>
+    <t>TC_SU_001</t>
+  </si>
+  <si>
+    <t>TC_SU_002</t>
+  </si>
+  <si>
+    <t>TC_SU_003</t>
+  </si>
+  <si>
+    <t>TC_SU_004</t>
+  </si>
+  <si>
+    <t>1. Mở ứng dụng
+2.Chọn màn hình account
+3.Chọn login
+4.Chọn tab signup</t>
+  </si>
+  <si>
+    <t>Kiểm tra khi bỏ trống vùng nhập đăng ký</t>
+  </si>
+  <si>
+    <t>Kiểm tra khi nhập trùng</t>
+  </si>
+  <si>
+    <t>Kiểm tra đăng ký thành công</t>
+  </si>
+  <si>
+    <t>Đã fix</t>
+  </si>
+  <si>
+    <t>Lỗi sai message trùng email</t>
+  </si>
+  <si>
+    <t>TC_C_001</t>
+  </si>
+  <si>
+    <t>TC_C_002</t>
+  </si>
+  <si>
+    <t>TC_C_003</t>
+  </si>
+  <si>
+    <t>TC_C_004</t>
+  </si>
+  <si>
+    <t>TC_C_005</t>
+  </si>
+  <si>
+    <t>TC_C_006</t>
+  </si>
+  <si>
+    <t>Kiểm tra cart có hiển thị đúng những sản phẩm được thêm không</t>
+  </si>
+  <si>
+    <t>1. Mở ứng dụng
+2.Thêm sản phẩm vào cart
+3. Mở màn hình cart</t>
+  </si>
+  <si>
+    <t>1. Chọn màn hình cart
+2.Chọn checkbox của 1 sản phẩm</t>
+  </si>
+  <si>
+    <t>Kiểm tra chức năng checkbox 1 sản phẩm trong cart</t>
+  </si>
+  <si>
+    <t>1. Chọn màn hình cart
+2.Chọn checkbox của select all</t>
+  </si>
+  <si>
+    <t>Chọn checkbox select all</t>
+  </si>
+  <si>
+    <t>Kiểm tra chức năng checkbox tất cả sản phẩm trong cart</t>
+  </si>
+  <si>
+    <t>1. Chọn màn hình cart
+2. Nhập số lượng tại mỗi sản phẩm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kiểm tra khi thay đổi số lượng </t>
+  </si>
+  <si>
+    <t>1. Chọn màn hình cart
+2. Chọn checkbox vào sản phẩm
+3. Nhấn delete</t>
+  </si>
+  <si>
+    <t>Kiểm tra xem chức năng xóa sản phẩm trong giỏ hàng</t>
+  </si>
+  <si>
+    <t>TC_C_007</t>
+  </si>
+  <si>
+    <t>TC_C_008</t>
+  </si>
+  <si>
+    <t>TC_C_009</t>
+  </si>
+  <si>
+    <t>TC_C_010</t>
+  </si>
+  <si>
+    <t>TC_C_011</t>
+  </si>
+  <si>
+    <t>1. Tại hộp thoại xác nhận chọn remove</t>
+  </si>
+  <si>
+    <t>Kiểm tra xác nhận xóa sản phẩm trong giỏ hàng</t>
+  </si>
+  <si>
+    <t>1. Tại hộp thoại xác nhận chọn cancel</t>
+  </si>
+  <si>
+    <t>Kiểm tra việc hủy xác nhận xóa sản phẩm</t>
+  </si>
+  <si>
+    <t>Kiểm tra button mua hàng</t>
+  </si>
+  <si>
+    <t>Kiểm tra chức năng đặt hàng</t>
+  </si>
+  <si>
+    <t>Kiểm tra chọn phương thức thanh toán</t>
+  </si>
+  <si>
+    <t>1. Chọn màn hình cart
+2. Chọn checkbox vào sản phẩm
+3. Nhấn buy</t>
+  </si>
+  <si>
+    <t>1. Tại màn hình đặt hàng nhấn Order</t>
+  </si>
+  <si>
+    <t>1. Tại màn hình chọn phương thức thanh toán chọn Cash</t>
+  </si>
+  <si>
+    <t>Đã đăng nhập, có sản phẩm trong cart</t>
+  </si>
+  <si>
+    <t>TC_CA_001</t>
+  </si>
+  <si>
+    <t>TC_CA_002</t>
+  </si>
+  <si>
+    <t>TC_CA_003</t>
+  </si>
+  <si>
+    <t>1. Mở ứng dụng
+2.Chọn màn hình category</t>
+  </si>
+  <si>
+    <t>Kiểm tra hiển thị đầy đủ các danh mục</t>
+  </si>
+  <si>
+    <t>Kiểm tra khi nhấn vào 1 danh mục</t>
+  </si>
+  <si>
+    <t>1. Tại màn hình category
+2.Chọn vào Bút viết</t>
+  </si>
+  <si>
+    <t>TC_A_001</t>
+  </si>
+  <si>
+    <t>TC_A_002</t>
+  </si>
+  <si>
+    <t>TC_A_003</t>
+  </si>
+  <si>
+    <t>TC_A_004</t>
+  </si>
+  <si>
+    <t>TC_A_005</t>
+  </si>
+  <si>
+    <t>TC_A_006</t>
+  </si>
+  <si>
+    <t>TC_A_007</t>
+  </si>
+  <si>
+    <t>Kiểm tra hiển thị danh sách địa chỉ</t>
+  </si>
+  <si>
+    <t>1. Mở ứng dụng
+2.Chọn màn hình account
+3. Chọn Address book</t>
+  </si>
+  <si>
+    <t>Kiểm tra thêm mới địa chỉ</t>
+  </si>
+  <si>
+    <t>1. Tại màn hình danh sách địa chỉ
+2.Chọn add new address
+3. Nhập input
+4. Chọn confirm</t>
+  </si>
+  <si>
+    <t>Kiểm tra xem chức năng xem danh sách các đơn hàng của người dùng</t>
+  </si>
+  <si>
+    <t>1. Người dùng ở trang account
+2.Người dùng chọn text "see all" ở mục your order hoặc nhấn biểu tượng</t>
+  </si>
+  <si>
+    <t>Kiểm tra chức năng thay đổi thông tin</t>
+  </si>
+  <si>
+    <t>1. Người dùng ở trang account
+2.Người dùng chọn edit profile
+3. Thay đổi thông tin
+4. Nhấn save</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kiểm tra xem chức năng thay đổi mật khẩu </t>
+  </si>
+  <si>
+    <t>1. Người dùng ở trang account
+2.Người dùng chọn change password
+3. Thay đổi thông tin
+4. Nhấn save</t>
+  </si>
+  <si>
+    <t>TC_SP_001</t>
+  </si>
+  <si>
+    <t>TC_SP_002</t>
+  </si>
+  <si>
+    <t>TC_SP_003</t>
+  </si>
+  <si>
+    <t>TC_SP_004</t>
+  </si>
+  <si>
+    <t>Kiểm tra hiện thị đúng các đơn hàng thuộc trách nhiệm của shipper hay không</t>
+  </si>
+  <si>
+    <t>1. Mở ứng dụng
+2.Đăng nhập</t>
+  </si>
+  <si>
+    <t>Kiểm tra chức năng xác nhận giao hàng thành công</t>
+  </si>
+  <si>
+    <t>1. Chọn đơn hàng
+2.Chọn xác nhận giao hàng
+3. Chọn OK trên hộp thoại</t>
+  </si>
+  <si>
+    <t>Kiểm tra xem chức năng hủy giao đơn hàng</t>
+  </si>
+  <si>
+    <t>1. Chọn đơn hàng
+2.Chọn hủy giao
+3. Chọn OK trên hộp thoại</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -328,8 +775,22 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="&quot;Times New Roman&quot;"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="&quot;Times New Roman&quot;"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -348,8 +809,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF333399"/>
+        <bgColor rgb="FF333399"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FFFF"/>
+        <bgColor rgb="FF00FFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -385,6 +858,98 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -393,7 +958,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -445,6 +1010,34 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -533,6 +1126,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>426720</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>314425</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3474720" y="0"/>
+          <a:ext cx="4764505" cy="10058400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -859,11 +1501,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView topLeftCell="A34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.5" customHeight="1"/>
   <cols>
     <col min="2" max="2" width="6.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.5546875" customWidth="1"/>
@@ -872,7 +1514,7 @@
     <col min="6" max="6" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" ht="13.2">
       <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
@@ -889,7 +1531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" ht="13.2">
       <c r="B3" s="4">
         <v>1</v>
       </c>
@@ -900,7 +1542,7 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="2:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" ht="13.2">
       <c r="B4" s="7">
         <v>1.1000000000000001</v>
       </c>
@@ -915,7 +1557,7 @@
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="2:6" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" ht="26.4">
       <c r="B5" s="7">
         <v>1.2</v>
       </c>
@@ -930,7 +1572,7 @@
       </c>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="2:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" ht="13.2">
       <c r="B6" s="7">
         <v>1.3</v>
       </c>
@@ -945,7 +1587,7 @@
       </c>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="2:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" ht="13.2">
       <c r="B7" s="4">
         <v>2</v>
       </c>
@@ -956,7 +1598,7 @@
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
     </row>
-    <row r="8" spans="2:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" ht="13.2">
       <c r="B8" s="9">
         <v>2.1</v>
       </c>
@@ -969,7 +1611,7 @@
       </c>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="2:6" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" ht="26.4">
       <c r="B9" s="9">
         <v>2.2000000000000002</v>
       </c>
@@ -984,7 +1626,7 @@
       </c>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="2:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" ht="13.2">
       <c r="B10" s="9">
         <v>2.2999999999999998</v>
       </c>
@@ -999,7 +1641,7 @@
       </c>
       <c r="F10" s="10"/>
     </row>
-    <row r="11" spans="2:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" ht="13.2">
       <c r="B11" s="9">
         <v>2.2999999999999998</v>
       </c>
@@ -1014,7 +1656,7 @@
       </c>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="2:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" ht="13.2">
       <c r="B12" s="4">
         <v>3</v>
       </c>
@@ -1025,7 +1667,7 @@
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
     </row>
-    <row r="13" spans="2:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" ht="13.2">
       <c r="B13" s="9">
         <v>3.1</v>
       </c>
@@ -1040,7 +1682,7 @@
       </c>
       <c r="F13" s="17"/>
     </row>
-    <row r="14" spans="2:6" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" ht="26.4">
       <c r="B14" s="9">
         <v>3.2</v>
       </c>
@@ -1055,7 +1697,7 @@
       </c>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="2:6" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" ht="39.6">
       <c r="B15" s="9">
         <v>3.3</v>
       </c>
@@ -1070,7 +1712,7 @@
       </c>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="2:6" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" ht="39.6">
       <c r="B16" s="9">
         <v>3.4</v>
       </c>
@@ -1085,7 +1727,7 @@
       </c>
       <c r="F16" s="11"/>
     </row>
-    <row r="17" spans="2:6" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" ht="39.6">
       <c r="B17" s="9">
         <v>3.5</v>
       </c>
@@ -1100,7 +1742,7 @@
       </c>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="2:6" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" ht="26.4">
       <c r="B18" s="9">
         <v>3.6</v>
       </c>
@@ -1115,7 +1757,7 @@
       </c>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="2:6" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" ht="26.4">
       <c r="B19" s="9">
         <v>3.7</v>
       </c>
@@ -1130,7 +1772,7 @@
       </c>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="2:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" ht="13.2">
       <c r="B20" s="9">
         <v>3.8</v>
       </c>
@@ -1145,7 +1787,7 @@
       </c>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="2:6" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6" ht="26.4">
       <c r="B21" s="9">
         <v>3.9</v>
       </c>
@@ -1160,7 +1802,7 @@
       </c>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="2:6" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" ht="39.6">
       <c r="B22" s="9">
         <v>4</v>
       </c>
@@ -1175,7 +1817,7 @@
       </c>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="2:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6" ht="13.2">
       <c r="B23" s="9">
         <v>4.0999999999999996</v>
       </c>
@@ -1190,7 +1832,7 @@
       </c>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" ht="13.2">
       <c r="B24" s="4">
         <v>4</v>
       </c>
@@ -1201,7 +1843,7 @@
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
     </row>
-    <row r="25" spans="2:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6" ht="13.2">
       <c r="B25" s="9">
         <v>4.0999999999999996</v>
       </c>
@@ -1216,7 +1858,7 @@
       </c>
       <c r="F25" s="17"/>
     </row>
-    <row r="26" spans="2:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:6" ht="13.2">
       <c r="B26" s="9">
         <v>4.2</v>
       </c>
@@ -1229,7 +1871,7 @@
       </c>
       <c r="F26" s="17"/>
     </row>
-    <row r="27" spans="2:6" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:6" ht="26.4">
       <c r="B27" s="9">
         <v>4.3</v>
       </c>
@@ -1244,7 +1886,7 @@
       </c>
       <c r="F27" s="17"/>
     </row>
-    <row r="28" spans="2:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:6" ht="13.2">
       <c r="B28" s="4">
         <v>5</v>
       </c>
@@ -1255,7 +1897,7 @@
       <c r="E28" s="8"/>
       <c r="F28" s="8"/>
     </row>
-    <row r="29" spans="2:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:6" ht="13.2">
       <c r="B29" s="9">
         <v>5.0999999999999996</v>
       </c>
@@ -1270,7 +1912,7 @@
       </c>
       <c r="F29" s="17"/>
     </row>
-    <row r="30" spans="2:6" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:6" ht="26.4">
       <c r="B30" s="9">
         <v>5.2</v>
       </c>
@@ -1285,7 +1927,7 @@
       </c>
       <c r="F30" s="17"/>
     </row>
-    <row r="31" spans="2:6" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:6" ht="26.4">
       <c r="B31" s="9">
         <v>5.3</v>
       </c>
@@ -1300,7 +1942,7 @@
       </c>
       <c r="F31" s="17"/>
     </row>
-    <row r="32" spans="2:6" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:6" ht="26.4">
       <c r="B32" s="9">
         <v>5.4</v>
       </c>
@@ -1313,7 +1955,7 @@
       </c>
       <c r="F32" s="17"/>
     </row>
-    <row r="33" spans="2:6" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:6" ht="26.4">
       <c r="B33" s="9">
         <v>5.5</v>
       </c>
@@ -1326,7 +1968,7 @@
       </c>
       <c r="F33" s="17"/>
     </row>
-    <row r="34" spans="2:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:6" ht="13.2">
       <c r="B34" s="9">
         <v>5.6</v>
       </c>
@@ -1341,7 +1983,7 @@
       </c>
       <c r="F34" s="17"/>
     </row>
-    <row r="35" spans="2:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:6" ht="13.2">
       <c r="B35" s="9">
         <v>5.7</v>
       </c>
@@ -1356,7 +1998,7 @@
       </c>
       <c r="F35" s="17"/>
     </row>
-    <row r="36" spans="2:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:6" ht="13.2">
       <c r="B36" s="4">
         <v>6</v>
       </c>
@@ -1367,7 +2009,7 @@
       <c r="E36" s="8"/>
       <c r="F36" s="8"/>
     </row>
-    <row r="37" spans="2:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:6" ht="13.2">
       <c r="B37" s="9">
         <v>6.1</v>
       </c>
@@ -1382,7 +2024,7 @@
       </c>
       <c r="F37" s="17"/>
     </row>
-    <row r="38" spans="2:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:6" ht="13.2">
       <c r="B38" s="9">
         <v>6.2</v>
       </c>
@@ -1395,7 +2037,7 @@
       </c>
       <c r="F38" s="17"/>
     </row>
-    <row r="39" spans="2:6" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:6" ht="26.4">
       <c r="B39" s="9">
         <v>6.3</v>
       </c>
@@ -1408,9 +2050,11 @@
       <c r="E39" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="F39" s="17"/>
-    </row>
-    <row r="40" spans="2:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="F39" s="17" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" ht="26.4">
       <c r="B40" s="9">
         <v>6.4</v>
       </c>
@@ -1423,7 +2067,7 @@
       </c>
       <c r="F40" s="17"/>
     </row>
-    <row r="41" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:6" ht="16.5" customHeight="1">
       <c r="B41" s="4">
         <v>7</v>
       </c>
@@ -1434,7 +2078,7 @@
       <c r="E41" s="8"/>
       <c r="F41" s="8"/>
     </row>
-    <row r="42" spans="2:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:6" ht="13.2">
       <c r="B42" s="9">
         <v>7.1</v>
       </c>
@@ -1449,7 +2093,7 @@
       </c>
       <c r="F42" s="17"/>
     </row>
-    <row r="43" spans="2:6" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:6" ht="39.6">
       <c r="B43" s="9">
         <v>7.2</v>
       </c>
@@ -1458,11 +2102,11 @@
       </c>
       <c r="D43" s="17"/>
       <c r="E43" s="14" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="F43" s="17"/>
     </row>
-    <row r="44" spans="2:6" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:6" ht="26.4">
       <c r="B44" s="9">
         <v>7.3</v>
       </c>
@@ -1471,7 +2115,7 @@
       </c>
       <c r="D44" s="17"/>
       <c r="E44" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F44" s="17"/>
     </row>
@@ -1479,4 +2123,2883 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2"/>
+  <cols>
+    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1"/>
+    <col min="6" max="6" width="26.21875" customWidth="1"/>
+    <col min="7" max="7" width="26.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="13.2" customHeight="1">
+      <c r="A1" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="J1" s="21"/>
+      <c r="K1" s="19" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="27.6">
+      <c r="A2" s="22"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="J2" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="K2" s="23"/>
+    </row>
+    <row r="3" spans="1:11" ht="13.2" customHeight="1">
+      <c r="A3" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="23"/>
+    </row>
+    <row r="4" spans="1:11" ht="39.6">
+      <c r="A4" s="27" t="s">
+        <v>104</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="D4" s="27"/>
+      <c r="E4" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="G4" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
+    </row>
+    <row r="5" spans="1:11" ht="39.6">
+      <c r="A5" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="D5" s="27"/>
+      <c r="E5" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="G5" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="27"/>
+    </row>
+    <row r="6" spans="1:11" ht="39.6">
+      <c r="A6" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="D6" s="27"/>
+      <c r="E6" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="G6" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
+    </row>
+    <row r="7" spans="1:11" ht="39.6">
+      <c r="A7" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="G7" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
+    </row>
+    <row r="8" spans="1:11" ht="39.6">
+      <c r="A8" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>118</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="G8" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="27"/>
+    </row>
+    <row r="9" spans="1:11" ht="52.8">
+      <c r="A9" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="B9" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>125</v>
+      </c>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="F9" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="G9" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="27"/>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="27"/>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="27"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="27"/>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="27"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="27"/>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="27"/>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="27"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="27"/>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="27"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="27"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="27"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="27"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="27"/>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="27"/>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" s="27"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27"/>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="27"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="27"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2"/>
+  <cols>
+    <col min="1" max="1" width="11.109375" customWidth="1"/>
+    <col min="2" max="2" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1"/>
+    <col min="6" max="6" width="26.21875" customWidth="1"/>
+    <col min="7" max="7" width="26.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="13.2" customHeight="1">
+      <c r="A1" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="J1" s="21"/>
+      <c r="K1" s="19" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="27.6">
+      <c r="A2" s="22"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="J2" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="K2" s="23"/>
+    </row>
+    <row r="3" spans="1:11" ht="13.2" customHeight="1">
+      <c r="A3" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="23"/>
+    </row>
+    <row r="4" spans="1:11" ht="39.6">
+      <c r="A4" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>134</v>
+      </c>
+      <c r="D4" s="27"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="27" t="s">
+        <v>135</v>
+      </c>
+      <c r="G4" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
+    </row>
+    <row r="5" spans="1:11" ht="39.6">
+      <c r="A5" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>136</v>
+      </c>
+      <c r="D5" s="27"/>
+      <c r="E5" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>137</v>
+      </c>
+      <c r="G5" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="27"/>
+    </row>
+    <row r="6" spans="1:11" ht="39.6">
+      <c r="A6" s="27" t="s">
+        <v>131</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="D6" s="27"/>
+      <c r="E6" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="G6" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
+    </row>
+    <row r="7" spans="1:11" ht="39.6">
+      <c r="A7" s="27" t="s">
+        <v>132</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27" t="s">
+        <v>135</v>
+      </c>
+      <c r="G7" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
+    </row>
+    <row r="8" spans="1:11" ht="92.4">
+      <c r="A8" s="27" t="s">
+        <v>133</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>139</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>143</v>
+      </c>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27" t="s">
+        <v>142</v>
+      </c>
+      <c r="F8" s="27" t="s">
+        <v>140</v>
+      </c>
+      <c r="G8" s="27" t="s">
+        <v>141</v>
+      </c>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="27"/>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="27"/>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="27"/>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="27"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="27"/>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="27"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="27"/>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="27"/>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="27"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="27"/>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="27"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="27"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="27"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="27"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="27"/>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="27"/>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" s="27"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27"/>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="27"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="27"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2"/>
+  <cols>
+    <col min="1" max="1" width="11.109375" customWidth="1"/>
+    <col min="2" max="2" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1"/>
+    <col min="6" max="6" width="26.21875" customWidth="1"/>
+    <col min="7" max="7" width="26.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="13.2" customHeight="1">
+      <c r="A1" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="J1" s="21"/>
+      <c r="K1" s="19" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="27.6">
+      <c r="A2" s="22"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="J2" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="K2" s="23"/>
+    </row>
+    <row r="3" spans="1:11" ht="13.2" customHeight="1">
+      <c r="A3" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="23"/>
+    </row>
+    <row r="4" spans="1:11" ht="52.8">
+      <c r="A4" s="27" t="s">
+        <v>144</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>149</v>
+      </c>
+      <c r="D4" s="27"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="27" t="s">
+        <v>148</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
+    </row>
+    <row r="5" spans="1:11" ht="66">
+      <c r="A5" s="27" t="s">
+        <v>145</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="D5" s="27"/>
+      <c r="E5" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>148</v>
+      </c>
+      <c r="G5" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="H5" s="27" t="s">
+        <v>153</v>
+      </c>
+      <c r="I5" s="27"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="27" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="52.8">
+      <c r="A6" s="27" t="s">
+        <v>146</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="D6" s="27"/>
+      <c r="E6" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="27" t="s">
+        <v>148</v>
+      </c>
+      <c r="G6" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
+    </row>
+    <row r="7" spans="1:11" ht="52.8">
+      <c r="A7" s="27" t="s">
+        <v>147</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>151</v>
+      </c>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27" t="s">
+        <v>148</v>
+      </c>
+      <c r="G7" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="27"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="27"/>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="27"/>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="27"/>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="27"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="27"/>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="27"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="27"/>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="27"/>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="27"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="27"/>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="27"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="27"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="27"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="27"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="27"/>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="27"/>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" s="27"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27"/>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="27"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="27"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K21"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2"/>
+  <cols>
+    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1"/>
+    <col min="6" max="6" width="26.21875" customWidth="1"/>
+    <col min="7" max="7" width="26.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="13.2" customHeight="1">
+      <c r="A1" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="J1" s="21"/>
+      <c r="K1" s="19" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="27.6">
+      <c r="A2" s="22"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="J2" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="K2" s="23"/>
+    </row>
+    <row r="3" spans="1:11" ht="13.2" customHeight="1">
+      <c r="A3" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="23"/>
+    </row>
+    <row r="4" spans="1:11" ht="39.6">
+      <c r="A4" s="27" t="s">
+        <v>154</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>160</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" s="27" t="s">
+        <v>161</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
+    </row>
+    <row r="5" spans="1:11" ht="52.8">
+      <c r="A5" s="27" t="s">
+        <v>155</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>163</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>162</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="27"/>
+    </row>
+    <row r="6" spans="1:11" ht="39.6">
+      <c r="A6" s="27" t="s">
+        <v>156</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
+    </row>
+    <row r="7" spans="1:11" ht="52.8">
+      <c r="A7" s="27" t="s">
+        <v>157</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="F7" s="27" t="s">
+        <v>164</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
+    </row>
+    <row r="8" spans="1:11" ht="66">
+      <c r="A8" s="27" t="s">
+        <v>158</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>168</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="27" t="s">
+        <v>167</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="27"/>
+    </row>
+    <row r="9" spans="1:11" ht="52.8">
+      <c r="A9" s="27" t="s">
+        <v>159</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>170</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="27" t="s">
+        <v>169</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="27"/>
+    </row>
+    <row r="10" spans="1:11" ht="39.6">
+      <c r="A10" s="27" t="s">
+        <v>171</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>177</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="27" t="s">
+        <v>176</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="27"/>
+    </row>
+    <row r="11" spans="1:11" ht="39.6">
+      <c r="A11" s="27" t="s">
+        <v>172</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>179</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="27" t="s">
+        <v>178</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="27"/>
+    </row>
+    <row r="12" spans="1:11" ht="52.8">
+      <c r="A12" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="D12" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="27" t="s">
+        <v>183</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="27"/>
+    </row>
+    <row r="13" spans="1:11" ht="52.8">
+      <c r="A13" s="27" t="s">
+        <v>174</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="27" t="s">
+        <v>181</v>
+      </c>
+      <c r="D13" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="H13" s="27"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="27"/>
+    </row>
+    <row r="14" spans="1:11" ht="39.6">
+      <c r="A14" s="27" t="s">
+        <v>175</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="27" t="s">
+        <v>182</v>
+      </c>
+      <c r="D14" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="27"/>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="27"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="27"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="27"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="27"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="27"/>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="27"/>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" s="27"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27"/>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="27"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="27"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2"/>
+  <cols>
+    <col min="1" max="1" width="10.88671875" customWidth="1"/>
+    <col min="2" max="2" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1"/>
+    <col min="6" max="6" width="26.21875" customWidth="1"/>
+    <col min="7" max="7" width="26.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="13.2" customHeight="1">
+      <c r="A1" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="J1" s="21"/>
+      <c r="K1" s="19" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="27.6">
+      <c r="A2" s="22"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="J2" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="K2" s="23"/>
+    </row>
+    <row r="3" spans="1:11" ht="13.2" customHeight="1">
+      <c r="A3" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="23"/>
+    </row>
+    <row r="4" spans="1:11" ht="26.4">
+      <c r="A4" s="27" t="s">
+        <v>187</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>191</v>
+      </c>
+      <c r="D4" s="27"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="27" t="s">
+        <v>190</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
+    </row>
+    <row r="5" spans="1:11" ht="26.4">
+      <c r="A5" s="27" t="s">
+        <v>188</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>192</v>
+      </c>
+      <c r="D5" s="27"/>
+      <c r="E5" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>193</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="27"/>
+    </row>
+    <row r="6" spans="1:11" ht="39.6">
+      <c r="A6" s="27" t="s">
+        <v>189</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="D6" s="27"/>
+      <c r="E6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="27"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="27"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="27"/>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="27"/>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="27"/>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="27"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="27"/>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="27"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="27"/>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="27"/>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="27"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="27"/>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="27"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="27"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="27"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="27"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="27"/>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="27"/>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" s="27"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27"/>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="27"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="27"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2"/>
+  <cols>
+    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1"/>
+    <col min="6" max="6" width="26.21875" customWidth="1"/>
+    <col min="7" max="7" width="26.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="13.2" customHeight="1">
+      <c r="A1" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="J1" s="21"/>
+      <c r="K1" s="19" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="27.6">
+      <c r="A2" s="22"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="J2" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="K2" s="23"/>
+    </row>
+    <row r="3" spans="1:11" ht="13.2" customHeight="1">
+      <c r="A3" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="23"/>
+    </row>
+    <row r="4" spans="1:11" ht="39.6">
+      <c r="A4" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>201</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" s="27" t="s">
+        <v>202</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
+    </row>
+    <row r="5" spans="1:11" ht="66">
+      <c r="A5" s="27" t="s">
+        <v>195</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>203</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>204</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="27"/>
+    </row>
+    <row r="6" spans="1:11" ht="39.6">
+      <c r="A6" s="27" t="s">
+        <v>196</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
+    </row>
+    <row r="7" spans="1:11" ht="66">
+      <c r="A7" s="27" t="s">
+        <v>197</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>205</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27" t="s">
+        <v>206</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
+    </row>
+    <row r="8" spans="1:11" ht="66">
+      <c r="A8" s="27" t="s">
+        <v>198</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>207</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27" t="s">
+        <v>208</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="27"/>
+    </row>
+    <row r="9" spans="1:11" ht="79.2">
+      <c r="A9" s="27" t="s">
+        <v>199</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>209</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="F9" s="27" t="s">
+        <v>210</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="27"/>
+    </row>
+    <row r="10" spans="1:11" ht="79.2">
+      <c r="A10" s="27" t="s">
+        <v>200</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>209</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="F10" s="27" t="s">
+        <v>210</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="27"/>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="27"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="27"/>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="27"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="27"/>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="27"/>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="27"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="27"/>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="27"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="27"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="27"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="27"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="27"/>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="27"/>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" s="27"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27"/>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="27"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="27"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2"/>
+  <cols>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1"/>
+    <col min="6" max="6" width="26.21875" customWidth="1"/>
+    <col min="7" max="7" width="26.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="13.2" customHeight="1">
+      <c r="A1" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="J1" s="21"/>
+      <c r="K1" s="19" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="27.6">
+      <c r="A2" s="22"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="J2" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="K2" s="23"/>
+    </row>
+    <row r="3" spans="1:11" ht="13.2" customHeight="1">
+      <c r="A3" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="23"/>
+    </row>
+    <row r="4" spans="1:11" ht="26.4">
+      <c r="A4" s="27" t="s">
+        <v>211</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>215</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="27" t="s">
+        <v>216</v>
+      </c>
+      <c r="G4" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
+    </row>
+    <row r="5" spans="1:11" ht="39.6">
+      <c r="A5" s="27" t="s">
+        <v>212</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="27"/>
+    </row>
+    <row r="6" spans="1:11" ht="39.6">
+      <c r="A6" s="27" t="s">
+        <v>213</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>217</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="27" t="s">
+        <v>218</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
+    </row>
+    <row r="7" spans="1:11" ht="39.6">
+      <c r="A7" s="27" t="s">
+        <v>214</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>219</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="27"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="27"/>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="27"/>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="27"/>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="27"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="27"/>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="27"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="27"/>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="27"/>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="27"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="27"/>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="27"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="27"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="27"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="27"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="27"/>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="27"/>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" s="27"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27"/>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="27"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="27"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A63"/>
+  <sheetViews>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="P57" sqref="P57"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetData>
+    <row r="63" spans="1:1">
+      <c r="A63" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>